<commit_message>
✨ v2.0: Comissões automáticas + formatação brasileira + correções
</commit_message>
<xml_diff>
--- a/1-coleta/Template_Profissionais.xlsx
+++ b/1-coleta/Template_Profissionais.xlsx
@@ -1,37 +1,105 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="390" yWindow="615" windowWidth="19815" windowHeight="7110"/>
   </bookViews>
   <sheets>
-    <sheet name="Profissionais" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Profissionais" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+  <si>
+    <t>Nome_Profissional</t>
+  </si>
+  <si>
+    <t>Funcao</t>
+  </si>
+  <si>
+    <t>Tipo_Contrato</t>
+  </si>
+  <si>
+    <t>Percentual_Comissao</t>
+  </si>
+  <si>
+    <t>Salario_Fixo</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Data_Admissao</t>
+  </si>
+  <si>
+    <t>João Silva</t>
+  </si>
+  <si>
+    <t>Cabeleireiro</t>
+  </si>
+  <si>
+    <t>Percentual</t>
+  </si>
+  <si>
+    <t>Ativo</t>
+  </si>
+  <si>
+    <t>03/08/2025</t>
+  </si>
+  <si>
+    <t>Maria Santos</t>
+  </si>
+  <si>
+    <t>Manicure</t>
+  </si>
+  <si>
+    <t>20/10/2025</t>
+  </si>
+  <si>
+    <t>Pedro Oliveira</t>
+  </si>
+  <si>
+    <t>Barbeiro</t>
+  </si>
+  <si>
+    <t>08/12/2025</t>
+  </si>
+  <si>
+    <t>Ana Costa</t>
+  </si>
+  <si>
+    <t>Esteticista</t>
+  </si>
+  <si>
+    <t>Salario</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +114,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,186 +435,137 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Nome_Profissional</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Funcao</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Tipo_Contrato</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Percentual_Comissao</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Salario_Fixo</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Data_Admissao</t>
-        </is>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>João Silva</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Cabeleireiro</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Percentual</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
         <v>60</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>03/08/2025</t>
-        </is>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Maria Santos</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Manicure</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Percentual</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
         <v>50</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Pedro Oliveira</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Barbeiro</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Percentual</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
         <v>55</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>08/12/2025</t>
-        </is>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Ana Costa</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Esteticista</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Percentual</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>65</v>
-      </c>
-      <c r="E5" t="n">
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>60</v>
+      </c>
+      <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>08/12/2025</t>
-        </is>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>